<commit_message>
Click and change format duration on task item.
</commit_message>
<xml_diff>
--- a/проверка длительности.xlsx
+++ b/проверка длительности.xlsx
@@ -119,8 +119,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="dd/mm/yy\ h:mm;@"/>
-    <numFmt numFmtId="174" formatCode="dd/mm/yyyy\ h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ h:mm:ss"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -191,7 +191,7 @@
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -199,12 +199,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -213,15 +207,21 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -525,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,12 +536,11 @@
     <col min="3" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
     <col min="6" max="6" width="19.85546875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="3" customWidth="1"/>
+    <col min="8" max="10" width="11" customWidth="1"/>
     <col min="11" max="11" width="20.28515625" customWidth="1"/>
     <col min="12" max="12" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.85546875" style="15" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -551,584 +550,584 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="8" t="s">
+      <c r="H2" s="18"/>
+      <c r="I2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9" t="s">
+      <c r="J2" s="19"/>
+      <c r="K2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="M2" s="14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
+      <c r="A3" s="9">
         <f ca="1">RANDBETWEEN(DATE(2018,1,1),DATE(2018,11,30))</f>
-        <v>43321</v>
-      </c>
-      <c r="B3" s="12" t="str">
+        <v>43181</v>
+      </c>
+      <c r="B3" s="10" t="str">
         <f ca="1">TEXT(RAND(), "чч:мм:сс")</f>
-        <v>11:00:15</v>
-      </c>
-      <c r="C3" s="11">
+        <v>03:48:01</v>
+      </c>
+      <c r="C3" s="9">
         <v>43375</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="13" t="str">
+      <c r="E3" s="11" t="str">
         <f>TEXT(C3,"ДД.ММ.ГГГГ")&amp; " " &amp;TEXT(D3,"чч:мм:сс")</f>
         <v>02.10.2018 11:38:25</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="12">
         <f>(E3-$E$1)/(1/24/60/60)*1000</f>
         <v>1538480305000.0005</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="9">
         <f ca="1">RANDBETWEEN(DATE(2018,1,1),DATE(2018,11,30))</f>
-        <v>43252</v>
-      </c>
-      <c r="H3" s="12" t="str">
+        <v>43424</v>
+      </c>
+      <c r="H3" s="10" t="str">
         <f ca="1">TEXT(RAND(), "чч:мм:сс")</f>
-        <v>10:34:09</v>
-      </c>
-      <c r="I3" s="11">
+        <v>12:03:30</v>
+      </c>
+      <c r="I3" s="9">
         <v>43405</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="13" t="str">
+      <c r="K3" s="11" t="str">
         <f>TEXT(I3,"ДД.ММ.ГГГГ")&amp; " " &amp;TEXT(J3,"чч:мм:сс")</f>
         <v>01.11.2018 02:45:12</v>
       </c>
-      <c r="L3" s="14">
+      <c r="L3" s="12">
         <f>(K3-$E$1)/(1/24/60/60)*1000</f>
         <v>1541040312000</v>
       </c>
-      <c r="M3" s="17">
+      <c r="M3" s="15">
         <f>I3+J3-C3-D3</f>
         <v>29.629710648146659</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
+      <c r="A4" s="9">
         <f t="shared" ref="A4:A17" ca="1" si="0">RANDBETWEEN(DATE(2018,1,1),DATE(2018,11,30))</f>
-        <v>43247</v>
-      </c>
-      <c r="B4" s="12" t="str">
+        <v>43251</v>
+      </c>
+      <c r="B4" s="10" t="str">
         <f t="shared" ref="B4:B17" ca="1" si="1">TEXT(RAND(), "чч:мм:сс")</f>
-        <v>15:57:06</v>
-      </c>
-      <c r="C4" s="11">
+        <v>10:37:13</v>
+      </c>
+      <c r="C4" s="9">
         <v>43104</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="13" t="str">
+      <c r="E4" s="11" t="str">
         <f t="shared" ref="E4:E17" si="2">TEXT(C4,"ДД.ММ.ГГГГ")&amp; " " &amp;TEXT(D4,"чч:мм:сс")</f>
         <v>04.01.2018 14:07:17</v>
       </c>
-      <c r="F4" s="14">
-        <f t="shared" ref="F4:F17" si="3">(E4-$E$1)/(1/24/60/60)*1000</f>
+      <c r="F4" s="12">
+        <f t="shared" ref="F4:F16" si="3">(E4-$E$1)/(1/24/60/60)*1000</f>
         <v>1515074837000</v>
       </c>
-      <c r="G4" s="11">
-        <f t="shared" ref="G4:I17" ca="1" si="4">RANDBETWEEN(DATE(2018,1,1),DATE(2018,11,30))</f>
-        <v>43325</v>
-      </c>
-      <c r="H4" s="12" t="str">
-        <f t="shared" ref="H4:J17" ca="1" si="5">TEXT(RAND(), "чч:мм:сс")</f>
-        <v>16:25:25</v>
-      </c>
-      <c r="I4" s="11">
+      <c r="G4" s="9">
+        <f t="shared" ref="G4:G17" ca="1" si="4">RANDBETWEEN(DATE(2018,1,1),DATE(2018,11,30))</f>
+        <v>43180</v>
+      </c>
+      <c r="H4" s="10" t="str">
+        <f t="shared" ref="H4:H17" ca="1" si="5">TEXT(RAND(), "чч:мм:сс")</f>
+        <v>22:08:14</v>
+      </c>
+      <c r="I4" s="9">
         <v>43148</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="13" t="str">
+      <c r="K4" s="11" t="str">
         <f t="shared" ref="K4:K17" si="6">TEXT(I4,"ДД.ММ.ГГГГ")&amp; " " &amp;TEXT(J4,"чч:мм:сс")</f>
         <v>17.02.2018 10:13:39</v>
       </c>
-      <c r="L4" s="14">
+      <c r="L4" s="12">
         <f t="shared" ref="L4:L17" si="7">(K4-$E$1)/(1/24/60/60)*1000</f>
         <v>1518862419000.0002</v>
       </c>
-      <c r="M4" s="17">
+      <c r="M4" s="15">
         <f>I4+J4-C4-D4</f>
         <v>43.837754629631185</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+      <c r="A5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>43144</v>
-      </c>
-      <c r="B5" s="12" t="str">
+        <v>43154</v>
+      </c>
+      <c r="B5" s="10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>16:23:55</v>
-      </c>
-      <c r="C5" s="11">
+        <v>19:57:48</v>
+      </c>
+      <c r="C5" s="9">
         <v>43123</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="13" t="str">
+      <c r="E5" s="11" t="str">
         <f t="shared" si="2"/>
         <v>23.01.2018 21:25:40</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="12">
         <f t="shared" si="3"/>
         <v>1516742739999.9998</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>43137</v>
-      </c>
-      <c r="H5" s="12" t="str">
+        <v>43228</v>
+      </c>
+      <c r="H5" s="10" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>18:10:52</v>
-      </c>
-      <c r="I5" s="11">
+        <v>06:43:05</v>
+      </c>
+      <c r="I5" s="9">
         <v>43302</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="13" t="str">
+      <c r="K5" s="11" t="str">
         <f t="shared" si="6"/>
         <v>21.07.2018 23:39:15</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="12">
         <f t="shared" si="7"/>
         <v>1532216355000</v>
       </c>
-      <c r="M5" s="17">
+      <c r="M5" s="15">
         <f t="shared" ref="M5:M17" si="8">I5+J5-C5-D5</f>
         <v>179.09276620370403</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+      <c r="A6" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>43429</v>
-      </c>
-      <c r="B6" s="12" t="str">
+        <v>43378</v>
+      </c>
+      <c r="B6" s="10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>18:24:30</v>
-      </c>
-      <c r="C6" s="11">
+        <v>03:42:39</v>
+      </c>
+      <c r="C6" s="9">
         <v>43267</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="13" t="str">
+      <c r="E6" s="11" t="str">
         <f t="shared" si="2"/>
         <v>16.06.2018 16:29:54</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="12">
         <f t="shared" si="3"/>
         <v>1529166594000</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>43367</v>
-      </c>
-      <c r="H6" s="12" t="str">
+        <v>43382</v>
+      </c>
+      <c r="H6" s="10" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>13:46:20</v>
-      </c>
-      <c r="I6" s="11">
+        <v>03:04:39</v>
+      </c>
+      <c r="I6" s="9">
         <v>43323</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="13" t="str">
+      <c r="K6" s="11" t="str">
         <f t="shared" si="6"/>
         <v>11.08.2018 14:02:57</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="12">
         <f t="shared" si="7"/>
         <v>1533996177000.0002</v>
       </c>
-      <c r="M6" s="17">
+      <c r="M6" s="15">
         <f t="shared" si="8"/>
         <v>55.897951388889986</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
+      <c r="A7" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>43243</v>
-      </c>
-      <c r="B7" s="12" t="str">
+        <v>43415</v>
+      </c>
+      <c r="B7" s="10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>09:20:13</v>
-      </c>
-      <c r="C7" s="11">
+        <v>03:37:09</v>
+      </c>
+      <c r="C7" s="9">
         <v>43376</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="13" t="str">
+      <c r="E7" s="11" t="str">
         <f t="shared" si="2"/>
         <v>03.10.2018 20:17:05</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="12">
         <f t="shared" si="3"/>
         <v>1538597825000.0005</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>43392</v>
-      </c>
-      <c r="H7" s="12" t="str">
+        <v>43225</v>
+      </c>
+      <c r="H7" s="10" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>11:19:02</v>
-      </c>
-      <c r="I7" s="11">
+        <v>21:37:23</v>
+      </c>
+      <c r="I7" s="9">
         <v>43376</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="16">
         <v>0.88508101851851861</v>
       </c>
-      <c r="K7" s="13" t="str">
+      <c r="K7" s="11" t="str">
         <f t="shared" si="6"/>
         <v>03.10.2018 21:14:31</v>
       </c>
-      <c r="L7" s="14">
+      <c r="L7" s="12">
         <f t="shared" si="7"/>
         <v>1538601271000</v>
       </c>
-      <c r="M7" s="17">
+      <c r="M7" s="15">
         <f t="shared" si="8"/>
         <v>3.9884259258407773E-2</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
+      <c r="A8" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>43401</v>
-      </c>
-      <c r="B8" s="12" t="str">
+        <v>43344</v>
+      </c>
+      <c r="B8" s="10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>19:22:25</v>
-      </c>
-      <c r="C8" s="11">
+        <v>19:25:50</v>
+      </c>
+      <c r="C8" s="9">
         <v>43420</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="13" t="str">
+      <c r="E8" s="11" t="str">
         <f t="shared" si="2"/>
         <v>16.11.2018 00:59:12</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="12">
         <f t="shared" si="3"/>
         <v>1542329952000</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>43168</v>
-      </c>
-      <c r="H8" s="12" t="str">
+        <v>43104</v>
+      </c>
+      <c r="H8" s="10" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>12:23:56</v>
-      </c>
-      <c r="I8" s="11">
+        <v>04:39:38</v>
+      </c>
+      <c r="I8" s="9">
         <v>43420</v>
       </c>
-      <c r="J8" s="18">
-        <v>8.2777777777777783E-2</v>
-      </c>
-      <c r="K8" s="13" t="str">
+      <c r="J8" s="16">
+        <v>4.2708333333333327E-2</v>
+      </c>
+      <c r="K8" s="11" t="str">
         <f t="shared" si="6"/>
-        <v>16.11.2018 01:59:12</v>
-      </c>
-      <c r="L8" s="14">
+        <v>16.11.2018 01:01:30</v>
+      </c>
+      <c r="L8" s="12">
         <f t="shared" si="7"/>
-        <v>1542333552000.0005</v>
-      </c>
-      <c r="M8" s="17">
+        <v>1542330090000.0002</v>
+      </c>
+      <c r="M8" s="15">
         <f t="shared" si="8"/>
-        <v>4.1666666670191463E-2</v>
+        <v>1.5972222231923489E-3</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
+      <c r="A9" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>43267</v>
-      </c>
-      <c r="B9" s="12" t="str">
+        <v>43143</v>
+      </c>
+      <c r="B9" s="10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>15:01:52</v>
-      </c>
-      <c r="C9" s="11">
+        <v>04:34:20</v>
+      </c>
+      <c r="C9" s="9">
         <v>43373</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="13" t="str">
+      <c r="E9" s="11" t="str">
         <f t="shared" si="2"/>
         <v>30.09.2018 23:05:19</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="12">
         <f t="shared" si="3"/>
         <v>1538348719000</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>43266</v>
-      </c>
-      <c r="H9" s="12" t="str">
+        <v>43432</v>
+      </c>
+      <c r="H9" s="10" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>11:21:41</v>
-      </c>
-      <c r="I9" s="11">
+        <v>19:33:45</v>
+      </c>
+      <c r="I9" s="9">
         <v>43421</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="K9" s="13" t="str">
+      <c r="K9" s="11" t="str">
         <f t="shared" si="6"/>
         <v>17.11.2018 14:59:08</v>
       </c>
-      <c r="L9" s="14">
+      <c r="L9" s="12">
         <f t="shared" si="7"/>
         <v>1542466747999.9998</v>
       </c>
-      <c r="M9" s="17">
+      <c r="M9" s="15">
         <f t="shared" si="8"/>
         <v>47.662372685182739</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
+      <c r="A10" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>43129</v>
-      </c>
-      <c r="B10" s="12" t="str">
+        <v>43377</v>
+      </c>
+      <c r="B10" s="10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>23:16:51</v>
-      </c>
-      <c r="C10" s="11">
+        <v>12:36:04</v>
+      </c>
+      <c r="C10" s="9">
         <v>43422</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="13" t="str">
+      <c r="E10" s="11" t="str">
         <f t="shared" si="2"/>
         <v>18.11.2018 10:15:33</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="12">
         <f t="shared" si="3"/>
         <v>1542536132999.9998</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>43255</v>
-      </c>
-      <c r="H10" s="12" t="str">
+        <v>43356</v>
+      </c>
+      <c r="H10" s="10" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>22:05:16</v>
-      </c>
-      <c r="I10" s="11">
+        <v>01:13:05</v>
+      </c>
+      <c r="I10" s="9">
         <v>43423</v>
       </c>
-      <c r="J10" s="18">
+      <c r="J10" s="16">
         <v>0.42746527777777782</v>
       </c>
-      <c r="K10" s="13" t="str">
+      <c r="K10" s="11" t="str">
         <f t="shared" si="6"/>
         <v>19.11.2018 10:15:33</v>
       </c>
-      <c r="L10" s="14">
+      <c r="L10" s="12">
         <f t="shared" si="7"/>
         <v>1542622532999.9998</v>
       </c>
-      <c r="M10" s="17">
+      <c r="M10" s="15">
         <f t="shared" si="8"/>
         <v>0.99999999999712186</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
+      <c r="A11" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>43320</v>
-      </c>
-      <c r="B11" s="12" t="str">
+        <v>43295</v>
+      </c>
+      <c r="B11" s="10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>02:29:39</v>
-      </c>
-      <c r="C11" s="11">
+        <v>07:51:18</v>
+      </c>
+      <c r="C11" s="9">
         <v>43371</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="13" t="str">
+      <c r="E11" s="11" t="str">
         <f t="shared" si="2"/>
         <v>28.09.2018 06:59:59</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="12">
         <f t="shared" si="3"/>
         <v>1538117999000.0002</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>43235</v>
-      </c>
-      <c r="H11" s="12" t="str">
+        <v>43206</v>
+      </c>
+      <c r="H11" s="10" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>23:53:38</v>
-      </c>
-      <c r="I11" s="11">
+        <v>01:36:41</v>
+      </c>
+      <c r="I11" s="9">
         <v>43401</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="J11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="13" t="str">
+      <c r="K11" s="11" t="str">
         <f t="shared" si="6"/>
         <v>28.10.2018 06:59:59</v>
       </c>
-      <c r="L11" s="14">
+      <c r="L11" s="12">
         <f t="shared" si="7"/>
         <v>1540709999000.0002</v>
       </c>
-      <c r="M11" s="17">
+      <c r="M11" s="15">
         <f t="shared" si="8"/>
         <v>30.000000000002146</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
+      <c r="A12" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>43276</v>
-      </c>
-      <c r="B12" s="12" t="str">
+        <v>43370</v>
+      </c>
+      <c r="B12" s="10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>12:43:21</v>
-      </c>
-      <c r="C12" s="11">
+        <v>11:23:13</v>
+      </c>
+      <c r="C12" s="9">
         <v>43207</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="13" t="str">
+      <c r="E12" s="11" t="str">
         <f t="shared" si="2"/>
         <v>17.04.2018 07:59:58</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="12">
         <f t="shared" si="3"/>
         <v>1523951997999.9998</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>43143</v>
-      </c>
-      <c r="H12" s="12" t="str">
+        <v>43166</v>
+      </c>
+      <c r="H12" s="10" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>17:22:58</v>
-      </c>
-      <c r="I12" s="11">
+        <v>04:09:18</v>
+      </c>
+      <c r="I12" s="9">
         <v>43249</v>
       </c>
-      <c r="J12" s="12" t="s">
+      <c r="J12" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K12" s="13" t="str">
+      <c r="K12" s="11" t="str">
         <f t="shared" si="6"/>
         <v>29.05.2018 18:50:59</v>
       </c>
-      <c r="L12" s="14">
+      <c r="L12" s="12">
         <f t="shared" si="7"/>
         <v>1527619859000.0005</v>
       </c>
-      <c r="M12" s="17">
+      <c r="M12" s="15">
         <f t="shared" si="8"/>
         <v>42.452094907411009</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
+      <c r="A13" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>43250</v>
-      </c>
-      <c r="B13" s="12" t="str">
+        <v>43128</v>
+      </c>
+      <c r="B13" s="10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>18:31:46</v>
-      </c>
-      <c r="C13" s="11">
+        <v>22:55:27</v>
+      </c>
+      <c r="C13" s="9">
         <v>43342</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="13" t="str">
+      <c r="E13" s="11" t="str">
         <f t="shared" si="2"/>
         <v>30.08.2018 08:58:38</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="12">
         <f t="shared" si="3"/>
         <v>1535619517999.9998</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>43155</v>
-      </c>
-      <c r="H13" s="12" t="str">
+        <v>43314</v>
+      </c>
+      <c r="H13" s="10" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>19:46:42</v>
-      </c>
-      <c r="I13" s="11">
+        <v>06:16:04</v>
+      </c>
+      <c r="I13" s="9">
         <v>43420</v>
       </c>
-      <c r="J13" s="12" t="s">
+      <c r="J13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="13" t="str">
+      <c r="K13" s="11" t="str">
         <f t="shared" si="6"/>
         <v>16.11.2018 02:36:09</v>
       </c>
-      <c r="L13" s="14">
+      <c r="L13" s="12">
         <f t="shared" si="7"/>
         <v>1542335769000</v>
       </c>
-      <c r="M13" s="19">
+      <c r="M13" s="17">
         <f t="shared" si="8"/>
         <v>77.734386574073199</v>
       </c>
@@ -1137,51 +1136,51 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
+      <c r="A14" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>43281</v>
-      </c>
-      <c r="B14" s="12" t="str">
+        <v>43109</v>
+      </c>
+      <c r="B14" s="10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>14:50:00</v>
-      </c>
-      <c r="C14" s="11">
+        <v>08:17:40</v>
+      </c>
+      <c r="C14" s="9">
         <v>43158</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="13" t="str">
+      <c r="E14" s="11" t="str">
         <f t="shared" si="2"/>
         <v>27.02.2018 04:49:49</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="12">
         <f t="shared" si="3"/>
         <v>1519706989000.0002</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>43269</v>
-      </c>
-      <c r="H14" s="12" t="str">
+        <v>43131</v>
+      </c>
+      <c r="H14" s="10" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>12:58:35</v>
-      </c>
-      <c r="I14" s="11">
+        <v>15:55:58</v>
+      </c>
+      <c r="I14" s="9">
         <v>43306</v>
       </c>
-      <c r="J14" s="12" t="s">
+      <c r="J14" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="K14" s="13" t="str">
+      <c r="K14" s="11" t="str">
         <f t="shared" si="6"/>
         <v>25.07.2018 06:02:51</v>
       </c>
-      <c r="L14" s="14">
+      <c r="L14" s="12">
         <f t="shared" si="7"/>
         <v>1532498570999.9998</v>
       </c>
-      <c r="M14" s="19">
+      <c r="M14" s="17">
         <f t="shared" si="8"/>
         <v>148.05071759258959</v>
       </c>
@@ -1190,51 +1189,51 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="11">
+      <c r="A15" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>43132</v>
-      </c>
-      <c r="B15" s="12" t="str">
+        <v>43221</v>
+      </c>
+      <c r="B15" s="10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>18:40:17</v>
-      </c>
-      <c r="C15" s="11">
+        <v>02:35:21</v>
+      </c>
+      <c r="C15" s="9">
         <v>43300</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="13" t="str">
+      <c r="E15" s="11" t="str">
         <f t="shared" si="2"/>
         <v>19.07.2018 01:24:44</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="12">
         <f t="shared" si="3"/>
         <v>1531963484000.0005</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>43353</v>
-      </c>
-      <c r="H15" s="12" t="str">
+        <v>43259</v>
+      </c>
+      <c r="H15" s="10" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>11:20:48</v>
-      </c>
-      <c r="I15" s="11">
+        <v>17:15:54</v>
+      </c>
+      <c r="I15" s="9">
         <v>43395</v>
       </c>
-      <c r="J15" s="12" t="s">
+      <c r="J15" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="K15" s="13" t="str">
+      <c r="K15" s="11" t="str">
         <f t="shared" si="6"/>
         <v>22.10.2018 21:58:08</v>
       </c>
-      <c r="L15" s="14">
+      <c r="L15" s="12">
         <f t="shared" si="7"/>
         <v>1540245488000</v>
       </c>
-      <c r="M15" s="19">
+      <c r="M15" s="17">
         <f t="shared" si="8"/>
         <v>95.856527777777913</v>
       </c>
@@ -1243,51 +1242,51 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
+      <c r="A16" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>43222</v>
-      </c>
-      <c r="B16" s="12" t="str">
+        <v>43102</v>
+      </c>
+      <c r="B16" s="10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>13:58:55</v>
-      </c>
-      <c r="C16" s="11">
+        <v>21:51:50</v>
+      </c>
+      <c r="C16" s="9">
         <v>43286</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="13" t="str">
+      <c r="E16" s="11" t="str">
         <f t="shared" si="2"/>
         <v>05.07.2018 00:26:45</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="12">
         <f t="shared" si="3"/>
         <v>1530750405000</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>43169</v>
-      </c>
-      <c r="H16" s="12" t="str">
+        <v>43320</v>
+      </c>
+      <c r="H16" s="10" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>05:13:06</v>
-      </c>
-      <c r="I16" s="11">
+        <v>12:04:04</v>
+      </c>
+      <c r="I16" s="9">
         <v>43873</v>
       </c>
-      <c r="J16" s="12" t="s">
+      <c r="J16" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="K16" s="13" t="str">
+      <c r="K16" s="11" t="str">
         <f t="shared" si="6"/>
         <v>12.02.2020 09:34:45</v>
       </c>
-      <c r="L16" s="14">
+      <c r="L16" s="12">
         <f t="shared" si="7"/>
         <v>1581500085000.0002</v>
       </c>
-      <c r="M16" s="19">
+      <c r="M16" s="17">
         <f t="shared" si="8"/>
         <v>587.38055555555786</v>
       </c>
@@ -1296,51 +1295,51 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="11">
+      <c r="A17" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>43128</v>
-      </c>
-      <c r="B17" s="12" t="str">
+        <v>43270</v>
+      </c>
+      <c r="B17" s="10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>07:16:50</v>
-      </c>
-      <c r="C17" s="11">
+        <v>03:48:09</v>
+      </c>
+      <c r="C17" s="9">
         <v>43124</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="13" t="str">
+      <c r="E17" s="11" t="str">
         <f t="shared" si="2"/>
         <v>24.01.2018 01:56:05</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="12">
         <f>(E17-$E$1)/(1/24/60/60)*1000</f>
         <v>1516758965000</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>43392</v>
-      </c>
-      <c r="H17" s="12" t="str">
+        <v>43101</v>
+      </c>
+      <c r="H17" s="10" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>16:36:41</v>
-      </c>
-      <c r="I17" s="11">
+        <v>02:29:02</v>
+      </c>
+      <c r="I17" s="9">
         <v>43425</v>
       </c>
-      <c r="J17" s="12" t="s">
+      <c r="J17" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="K17" s="13" t="str">
+      <c r="K17" s="11" t="str">
         <f t="shared" si="6"/>
         <v>21.11.2018 10:48:15</v>
       </c>
-      <c r="L17" s="14">
+      <c r="L17" s="12">
         <f t="shared" si="7"/>
         <v>1542797295000.0002</v>
       </c>
-      <c r="M17" s="19">
+      <c r="M17" s="17">
         <f t="shared" si="8"/>
         <v>301.36956018518646</v>
       </c>

</xml_diff>

<commit_message>
Change dates on item task
</commit_message>
<xml_diff>
--- a/проверка длительности.xlsx
+++ b/проверка длительности.xlsx
@@ -189,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -222,6 +222,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -526,7 +530,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,11 +589,11 @@
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <f ca="1">RANDBETWEEN(DATE(2018,1,1),DATE(2018,11,30))</f>
-        <v>43181</v>
+        <v>43276</v>
       </c>
       <c r="B3" s="10" t="str">
         <f ca="1">TEXT(RAND(), "чч:мм:сс")</f>
-        <v>03:48:01</v>
+        <v>13:54:06</v>
       </c>
       <c r="C3" s="9">
         <v>43375</v>
@@ -607,11 +611,11 @@
       </c>
       <c r="G3" s="9">
         <f ca="1">RANDBETWEEN(DATE(2018,1,1),DATE(2018,11,30))</f>
-        <v>43424</v>
+        <v>43143</v>
       </c>
       <c r="H3" s="10" t="str">
         <f ca="1">TEXT(RAND(), "чч:мм:сс")</f>
-        <v>12:03:30</v>
+        <v>13:40:17</v>
       </c>
       <c r="I3" s="9">
         <v>43405</v>
@@ -635,11 +639,11 @@
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <f t="shared" ref="A4:A17" ca="1" si="0">RANDBETWEEN(DATE(2018,1,1),DATE(2018,11,30))</f>
-        <v>43251</v>
+        <v>43282</v>
       </c>
       <c r="B4" s="10" t="str">
         <f t="shared" ref="B4:B17" ca="1" si="1">TEXT(RAND(), "чч:мм:сс")</f>
-        <v>10:37:13</v>
+        <v>13:11:37</v>
       </c>
       <c r="C4" s="9">
         <v>43104</v>
@@ -657,11 +661,11 @@
       </c>
       <c r="G4" s="9">
         <f t="shared" ref="G4:G17" ca="1" si="4">RANDBETWEEN(DATE(2018,1,1),DATE(2018,11,30))</f>
-        <v>43180</v>
+        <v>43145</v>
       </c>
       <c r="H4" s="10" t="str">
         <f t="shared" ref="H4:H17" ca="1" si="5">TEXT(RAND(), "чч:мм:сс")</f>
-        <v>22:08:14</v>
+        <v>06:05:17</v>
       </c>
       <c r="I4" s="9">
         <v>43148</v>
@@ -685,11 +689,11 @@
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>43154</v>
+        <v>43103</v>
       </c>
       <c r="B5" s="10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>19:57:48</v>
+        <v>01:16:10</v>
       </c>
       <c r="C5" s="9">
         <v>43123</v>
@@ -707,11 +711,11 @@
       </c>
       <c r="G5" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>43228</v>
+        <v>43378</v>
       </c>
       <c r="H5" s="10" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>06:43:05</v>
+        <v>01:52:08</v>
       </c>
       <c r="I5" s="9">
         <v>43302</v>
@@ -735,11 +739,11 @@
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>43378</v>
+        <v>43203</v>
       </c>
       <c r="B6" s="10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>03:42:39</v>
+        <v>21:33:56</v>
       </c>
       <c r="C6" s="9">
         <v>43267</v>
@@ -757,11 +761,11 @@
       </c>
       <c r="G6" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>43382</v>
+        <v>43185</v>
       </c>
       <c r="H6" s="10" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>03:04:39</v>
+        <v>14:57:56</v>
       </c>
       <c r="I6" s="9">
         <v>43323</v>
@@ -785,11 +789,11 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>43415</v>
+        <v>43160</v>
       </c>
       <c r="B7" s="10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>03:37:09</v>
+        <v>12:28:58</v>
       </c>
       <c r="C7" s="9">
         <v>43376</v>
@@ -807,11 +811,11 @@
       </c>
       <c r="G7" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>43225</v>
+        <v>43103</v>
       </c>
       <c r="H7" s="10" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>21:37:23</v>
+        <v>12:34:56</v>
       </c>
       <c r="I7" s="9">
         <v>43376</v>
@@ -832,22 +836,22 @@
         <v>3.9884259258407773E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+    <row r="8" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>43344</v>
-      </c>
-      <c r="B8" s="10" t="str">
+        <v>43203</v>
+      </c>
+      <c r="B8" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>19:25:50</v>
-      </c>
-      <c r="C8" s="9">
+        <v>23:54:29</v>
+      </c>
+      <c r="C8" s="20">
         <v>43420</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="11" t="str">
+      <c r="E8" s="22" t="str">
         <f t="shared" si="2"/>
         <v>16.11.2018 00:59:12</v>
       </c>
@@ -855,21 +859,21 @@
         <f t="shared" si="3"/>
         <v>1542329952000</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>43104</v>
-      </c>
-      <c r="H8" s="10" t="str">
+        <v>43385</v>
+      </c>
+      <c r="H8" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>04:39:38</v>
-      </c>
-      <c r="I8" s="9">
+        <v>23:56:03</v>
+      </c>
+      <c r="I8" s="20">
         <v>43420</v>
       </c>
-      <c r="J8" s="16">
+      <c r="J8" s="23">
         <v>4.2708333333333327E-2</v>
       </c>
-      <c r="K8" s="11" t="str">
+      <c r="K8" s="22" t="str">
         <f t="shared" si="6"/>
         <v>16.11.2018 01:01:30</v>
       </c>
@@ -877,7 +881,7 @@
         <f t="shared" si="7"/>
         <v>1542330090000.0002</v>
       </c>
-      <c r="M8" s="15">
+      <c r="M8" s="17">
         <f t="shared" si="8"/>
         <v>1.5972222231923489E-3</v>
       </c>
@@ -885,11 +889,11 @@
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>43143</v>
+        <v>43356</v>
       </c>
       <c r="B9" s="10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>04:34:20</v>
+        <v>14:56:11</v>
       </c>
       <c r="C9" s="9">
         <v>43373</v>
@@ -907,11 +911,11 @@
       </c>
       <c r="G9" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>43432</v>
+        <v>43387</v>
       </c>
       <c r="H9" s="10" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>19:33:45</v>
+        <v>02:51:37</v>
       </c>
       <c r="I9" s="9">
         <v>43421</v>
@@ -935,11 +939,11 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>43377</v>
+        <v>43332</v>
       </c>
       <c r="B10" s="10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>12:36:04</v>
+        <v>08:31:39</v>
       </c>
       <c r="C10" s="9">
         <v>43422</v>
@@ -957,11 +961,11 @@
       </c>
       <c r="G10" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>43356</v>
+        <v>43418</v>
       </c>
       <c r="H10" s="10" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>01:13:05</v>
+        <v>16:02:52</v>
       </c>
       <c r="I10" s="9">
         <v>43423</v>
@@ -985,11 +989,11 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>43295</v>
+        <v>43142</v>
       </c>
       <c r="B11" s="10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>07:51:18</v>
+        <v>19:25:19</v>
       </c>
       <c r="C11" s="9">
         <v>43371</v>
@@ -1007,11 +1011,11 @@
       </c>
       <c r="G11" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>43206</v>
+        <v>43272</v>
       </c>
       <c r="H11" s="10" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>01:36:41</v>
+        <v>17:45:36</v>
       </c>
       <c r="I11" s="9">
         <v>43401</v>
@@ -1035,11 +1039,11 @@
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>43370</v>
+        <v>43220</v>
       </c>
       <c r="B12" s="10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>11:23:13</v>
+        <v>00:18:37</v>
       </c>
       <c r="C12" s="9">
         <v>43207</v>
@@ -1057,11 +1061,11 @@
       </c>
       <c r="G12" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>43166</v>
+        <v>43429</v>
       </c>
       <c r="H12" s="10" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>04:09:18</v>
+        <v>10:11:33</v>
       </c>
       <c r="I12" s="9">
         <v>43249</v>
@@ -1085,11 +1089,11 @@
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>43128</v>
+        <v>43258</v>
       </c>
       <c r="B13" s="10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>22:55:27</v>
+        <v>07:18:12</v>
       </c>
       <c r="C13" s="9">
         <v>43342</v>
@@ -1107,11 +1111,11 @@
       </c>
       <c r="G13" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>43314</v>
+        <v>43136</v>
       </c>
       <c r="H13" s="10" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>06:16:04</v>
+        <v>06:02:19</v>
       </c>
       <c r="I13" s="9">
         <v>43420</v>
@@ -1138,11 +1142,11 @@
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>43109</v>
+        <v>43425</v>
       </c>
       <c r="B14" s="10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>08:17:40</v>
+        <v>22:44:34</v>
       </c>
       <c r="C14" s="9">
         <v>43158</v>
@@ -1160,11 +1164,11 @@
       </c>
       <c r="G14" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>43131</v>
+        <v>43420</v>
       </c>
       <c r="H14" s="10" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>15:55:58</v>
+        <v>18:41:05</v>
       </c>
       <c r="I14" s="9">
         <v>43306</v>
@@ -1191,11 +1195,11 @@
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>43221</v>
+        <v>43209</v>
       </c>
       <c r="B15" s="10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>02:35:21</v>
+        <v>23:55:07</v>
       </c>
       <c r="C15" s="9">
         <v>43300</v>
@@ -1213,11 +1217,11 @@
       </c>
       <c r="G15" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>43259</v>
+        <v>43225</v>
       </c>
       <c r="H15" s="10" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>17:15:54</v>
+        <v>15:32:51</v>
       </c>
       <c r="I15" s="9">
         <v>43395</v>
@@ -1244,11 +1248,11 @@
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>43102</v>
+        <v>43170</v>
       </c>
       <c r="B16" s="10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>21:51:50</v>
+        <v>21:18:52</v>
       </c>
       <c r="C16" s="9">
         <v>43286</v>
@@ -1266,11 +1270,11 @@
       </c>
       <c r="G16" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>43320</v>
+        <v>43204</v>
       </c>
       <c r="H16" s="10" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>12:04:04</v>
+        <v>20:01:29</v>
       </c>
       <c r="I16" s="9">
         <v>43873</v>
@@ -1297,11 +1301,11 @@
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>43270</v>
+        <v>43360</v>
       </c>
       <c r="B17" s="10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>03:48:09</v>
+        <v>20:26:23</v>
       </c>
       <c r="C17" s="9">
         <v>43124</v>
@@ -1319,11 +1323,11 @@
       </c>
       <c r="G17" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>43101</v>
+        <v>43348</v>
       </c>
       <c r="H17" s="10" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>02:29:02</v>
+        <v>12:31:43</v>
       </c>
       <c r="I17" s="9">
         <v>43425</v>

</xml_diff>